<commit_message>
2023/05/21 Hotel 데이터 추가
</commit_message>
<xml_diff>
--- a/src/data/Restaurant.xlsx
+++ b/src/data/Restaurant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjh57\OneDrive\바탕 화면\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AB2BEC-C35E-4CE0-9C5C-1A076E02EB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4724222-D4A9-4054-9157-0F584B1AC617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{8F7EDF03-781A-4D27-BB2C-7820C407F434}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="807">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2449,6 +2449,29 @@
   </si>
   <si>
     <t>Al Ponte</t>
+  </si>
+  <si>
+    <t>country</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>British</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>French</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Italy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switzerland</t>
   </si>
 </sst>
 </file>
@@ -2827,10 +2850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96941643-5720-4192-8EF5-9F252C8907D2}">
-  <dimension ref="A1:H222"/>
+  <dimension ref="A1:I222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I192" sqref="I192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2839,7 +2862,7 @@
     <col min="2" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2864,8 +2887,11 @@
       <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I1" s="2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -2890,8 +2916,11 @@
       <c r="H2" s="2">
         <v>-0.48034363926180901</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I2" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2916,8 +2945,11 @@
       <c r="H3" s="2">
         <v>-7.7896866495301795E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I3" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -2942,8 +2974,11 @@
       <c r="H4" s="2">
         <v>-0.13401752192864599</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I4" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -2968,8 +3003,11 @@
       <c r="H5" s="2">
         <v>-0.117842164204867</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I5" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -2994,8 +3032,11 @@
       <c r="H6" s="2">
         <v>-0.15915864740094501</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I6" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>40</v>
       </c>
@@ -3020,8 +3061,11 @@
       <c r="H7" s="2">
         <v>-0.108545140072575</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I7" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -3046,8 +3090,11 @@
       <c r="H8" s="2">
         <v>-0.13908138703492301</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I8" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -3072,8 +3119,11 @@
       <c r="H9" s="2">
         <v>-0.15100818809007799</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I9" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>57</v>
       </c>
@@ -3098,8 +3148,11 @@
       <c r="H10" s="2">
         <v>-2.7399893221253699</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I10" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>62</v>
       </c>
@@ -3124,8 +3177,11 @@
       <c r="H11" s="2">
         <v>-0.13857754695217001</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I11" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>67</v>
       </c>
@@ -3150,8 +3206,11 @@
       <c r="H12" s="2">
         <v>-0.151412783301583</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I12" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>71</v>
       </c>
@@ -3176,8 +3235,11 @@
       <c r="H13" s="2">
         <v>-0.15336609729021899</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I13" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>75</v>
       </c>
@@ -3202,8 +3264,11 @@
       <c r="H14" s="2">
         <v>-2.24354886511661</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I14" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>79</v>
       </c>
@@ -3228,8 +3293,11 @@
       <c r="H15" s="2">
         <v>-2.2570146347955902</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I15" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>83</v>
       </c>
@@ -3254,8 +3322,11 @@
       <c r="H16" s="2">
         <v>-2.24033357275023</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I16" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>87</v>
       </c>
@@ -3280,8 +3351,11 @@
       <c r="H17" s="2">
         <v>-2.23138719104197</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I17" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>92</v>
       </c>
@@ -3306,8 +3380,11 @@
       <c r="H18" s="2">
         <v>-2.2389226597413301</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I18" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>97</v>
       </c>
@@ -3332,8 +3409,11 @@
       <c r="H19" s="2">
         <v>-2.22753318929868</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I19" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>101</v>
       </c>
@@ -3358,8 +3438,11 @@
       <c r="H20" s="2">
         <v>-3.1997841978620398</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I20" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>105</v>
       </c>
@@ -3384,8 +3467,11 @@
       <c r="H21" s="2">
         <v>-3.1937119551949</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I21" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>110</v>
       </c>
@@ -3410,8 +3496,11 @@
       <c r="H22" s="2">
         <v>-3.2912082139746701</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I22" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>114</v>
       </c>
@@ -3436,8 +3525,11 @@
       <c r="H23" s="2">
         <v>-3.1848417967291098</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I23" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>119</v>
       </c>
@@ -3462,8 +3554,11 @@
       <c r="H24" s="2">
         <v>-3.2442350646515998</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I24" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>124</v>
       </c>
@@ -3488,8 +3583,11 @@
       <c r="H25" s="2">
         <v>-3.1996818267676099</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I25" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>128</v>
       </c>
@@ -3514,8 +3612,11 @@
       <c r="H26" s="2">
         <v>-1.2357005904198199</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I26" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>132</v>
       </c>
@@ -3540,8 +3641,11 @@
       <c r="H27" s="2">
         <v>-1.23299190189715</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I27" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>137</v>
       </c>
@@ -3566,8 +3670,11 @@
       <c r="H28" s="2">
         <v>-1.2356917019158</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I28" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>142</v>
       </c>
@@ -3592,8 +3699,11 @@
       <c r="H29" s="2">
         <v>-1.2305401414377299</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I29" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>147</v>
       </c>
@@ -3618,8 +3728,11 @@
       <c r="H30" s="2">
         <v>-1.2563078799907199</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I30" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>151</v>
       </c>
@@ -3644,8 +3757,11 @@
       <c r="H31" s="2">
         <v>-1.15509490685978</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I31" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>156</v>
       </c>
@@ -3670,8 +3786,11 @@
       <c r="H33" s="2">
         <v>2.3363434453680099</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I33" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>160</v>
       </c>
@@ -3696,8 +3815,11 @@
       <c r="H34" s="2">
         <v>2.3416329699245999</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I34" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>164</v>
       </c>
@@ -3722,8 +3844,11 @@
       <c r="H35" s="2">
         <v>2.2883787984713702</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I35" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>168</v>
       </c>
@@ -3748,8 +3873,11 @@
       <c r="H36" s="2">
         <v>2.3788953171439302</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I36" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
         <v>172</v>
       </c>
@@ -3774,8 +3902,11 @@
       <c r="H37" s="2">
         <v>2.3298240377397499</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I37" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>176</v>
       </c>
@@ -3800,8 +3931,11 @@
       <c r="H38" s="2">
         <v>2.3434316464567</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I38" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>180</v>
       </c>
@@ -3826,8 +3960,11 @@
       <c r="H40" s="2">
         <v>4.8263198304045103</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I40" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
         <v>185</v>
       </c>
@@ -3852,8 +3989,11 @@
       <c r="H41" s="2">
         <v>4.8292259387700502</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I41" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
         <v>188</v>
       </c>
@@ -3878,8 +4018,11 @@
       <c r="H42" s="2">
         <v>4.8552942271792299</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I42" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
         <v>192</v>
       </c>
@@ -3904,8 +4047,11 @@
       <c r="H43" s="2">
         <v>4.8306594067554798</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I43" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
         <v>196</v>
       </c>
@@ -3930,8 +4076,11 @@
       <c r="H44" s="2">
         <v>4.8556004167253199</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I44" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
         <v>198</v>
       </c>
@@ -3956,8 +4105,11 @@
       <c r="H45" s="2">
         <v>4.8318161224950504</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I45" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
         <v>204</v>
       </c>
@@ -3982,8 +4134,11 @@
       <c r="H47" s="2">
         <v>5.3739070383865402</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I47" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
         <v>209</v>
       </c>
@@ -4008,8 +4163,11 @@
       <c r="H48" s="2">
         <v>5.37354299665716</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I48" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>214</v>
       </c>
@@ -4034,8 +4192,11 @@
       <c r="H49" s="2">
         <v>5.35529617525654</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I49" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
         <v>220</v>
       </c>
@@ -4060,8 +4221,11 @@
       <c r="H50" s="2">
         <v>5.3755639584588204</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I50" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
         <v>225</v>
       </c>
@@ -4086,8 +4250,11 @@
       <c r="H51" s="2">
         <v>5.3888255822895497</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I51" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
         <v>230</v>
       </c>
@@ -4112,8 +4279,11 @@
       <c r="H52" s="2">
         <v>5.3653098838013902</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I52" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>234</v>
       </c>
@@ -4138,8 +4308,11 @@
       <c r="H54" s="2">
         <v>7.2649395333209599</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I54" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
         <v>238</v>
       </c>
@@ -4164,8 +4337,11 @@
       <c r="H55" s="2">
         <v>7.26472031677591</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I55" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
         <v>242</v>
       </c>
@@ -4190,8 +4366,11 @@
       <c r="H56" s="2">
         <v>7.2835787890914103</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I56" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
         <v>247</v>
       </c>
@@ -4216,8 +4395,11 @@
       <c r="H57" s="2">
         <v>7.2702510376656999</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I57" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
         <v>251</v>
       </c>
@@ -4242,8 +4424,11 @@
       <c r="H58" s="2">
         <v>7.2702360953456102</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I58" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
         <v>257</v>
       </c>
@@ -4268,8 +4453,11 @@
       <c r="H59" s="2">
         <v>7.2581661567904003</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I59" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
         <v>263</v>
       </c>
@@ -4294,8 +4482,11 @@
       <c r="H61" s="2">
         <v>1.4509886576575799</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I61" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
         <v>268</v>
       </c>
@@ -4320,8 +4511,11 @@
       <c r="H62" s="2">
         <v>1.451211185002</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I62" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
         <v>271</v>
       </c>
@@ -4346,8 +4540,11 @@
       <c r="H63" s="2">
         <v>1.4568247027160801</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I63" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
         <v>275</v>
       </c>
@@ -4372,8 +4569,11 @@
       <c r="H64" s="2">
         <v>1.4097535139681101</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I64" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
         <v>280</v>
       </c>
@@ -4398,8 +4598,11 @@
       <c r="H65" s="2">
         <v>1.4483319887072801</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I65" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
         <v>284</v>
       </c>
@@ -4424,8 +4627,11 @@
       <c r="H66" s="2">
         <v>1.4535164648097501</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I66" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
         <v>288</v>
       </c>
@@ -4450,8 +4656,11 @@
       <c r="H68" s="2">
         <v>-1.55489328668452</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I68" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
         <v>291</v>
       </c>
@@ -4476,8 +4685,11 @@
       <c r="H69" s="2">
         <v>-1.5633347308510499</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I69" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
         <v>295</v>
       </c>
@@ -4502,8 +4714,11 @@
       <c r="H70" s="2">
         <v>-1.5551411027800599</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I70" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
         <v>300</v>
       </c>
@@ -4528,8 +4743,11 @@
       <c r="H71" s="2">
         <v>-1.6263398731709799</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I71" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
         <v>304</v>
       </c>
@@ -4554,8 +4772,11 @@
       <c r="H72" s="2">
         <v>-1.5564803855049201</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I72" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
         <v>306</v>
       </c>
@@ -4580,8 +4801,11 @@
       <c r="H73" s="2">
         <v>-1.55484058299676</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I73" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
         <v>309</v>
       </c>
@@ -4606,8 +4830,11 @@
       <c r="H75" s="2">
         <v>7.7390286827598196</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I75" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
         <v>311</v>
       </c>
@@ -4632,8 +4859,11 @@
       <c r="H76" s="2">
         <v>7.7532634533529698</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I76" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
         <v>314</v>
       </c>
@@ -4658,8 +4888,11 @@
       <c r="H77" s="2">
         <v>7.7664660506281598</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I77" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
         <v>318</v>
       </c>
@@ -4684,8 +4917,11 @@
       <c r="H78" s="2">
         <v>7.7701250276703702</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I78" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
         <v>321</v>
       </c>
@@ -4710,8 +4946,11 @@
       <c r="H79" s="2">
         <v>7.7460975479713401</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I79" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
         <v>325</v>
       </c>
@@ -4736,8 +4975,11 @@
       <c r="H80" s="2">
         <v>7.7821740049657899</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I80" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
         <v>331</v>
       </c>
@@ -4762,8 +5004,11 @@
       <c r="H82" s="2">
         <v>-3.6682960679842598</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I82" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
         <v>335</v>
       </c>
@@ -4788,8 +5033,11 @@
       <c r="H83" s="2">
         <v>-3.70173236680519</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I83" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
         <v>339</v>
       </c>
@@ -4814,8 +5062,11 @@
       <c r="H84" s="2">
         <v>-3.7096281343299302</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I84" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
         <v>344</v>
       </c>
@@ -4840,8 +5091,11 @@
       <c r="H85" s="2">
         <v>-3.7016023316128499</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I85" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
         <v>348</v>
       </c>
@@ -4866,8 +5120,11 @@
       <c r="H86" s="2">
         <v>-3.5787300945441101</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I86" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
         <v>352</v>
       </c>
@@ -4892,8 +5149,11 @@
       <c r="H87" s="2">
         <v>-3.6707849399254</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I87" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
         <v>356</v>
       </c>
@@ -4918,8 +5178,11 @@
       <c r="H89" s="2">
         <v>2.2049049978236899</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I89" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
         <v>360</v>
       </c>
@@ -4944,8 +5207,11 @@
       <c r="H90" s="2">
         <v>2.1536709749220302</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I90" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
         <v>364</v>
       </c>
@@ -4970,8 +5236,11 @@
       <c r="H91" s="2">
         <v>2.15629821696665</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I91" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
         <v>369</v>
       </c>
@@ -4996,8 +5265,11 @@
       <c r="H92" s="2">
         <v>2.1734482015748</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I92" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
         <v>373</v>
       </c>
@@ -5022,8 +5294,11 @@
       <c r="H93" s="2">
         <v>2.2045564216652198</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I93" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
         <v>377</v>
       </c>
@@ -5048,8 +5323,11 @@
       <c r="H94" s="2">
         <v>2.1638690496000299</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I94" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
         <v>381</v>
       </c>
@@ -5074,8 +5352,11 @@
       <c r="H96" s="2">
         <v>-0.364813000671521</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I96" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
         <v>384</v>
       </c>
@@ -5100,8 +5381,11 @@
       <c r="H97" s="2">
         <v>-0.36514476528336998</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I97" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
         <v>388</v>
       </c>
@@ -5126,8 +5410,11 @@
       <c r="H98" s="2">
         <v>-0.37113390171985</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I98" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
         <v>393</v>
       </c>
@@ -5152,8 +5439,11 @@
       <c r="H99" s="2">
         <v>-0.31831328079152599</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I99" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
         <v>397</v>
       </c>
@@ -5178,8 +5468,11 @@
       <c r="H100" s="2">
         <v>-0.37807226775535202</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I100" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
         <v>401</v>
       </c>
@@ -5204,8 +5497,11 @@
       <c r="H101" s="2">
         <v>-0.37642597035772102</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I101" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
         <v>405</v>
       </c>
@@ -5230,8 +5526,11 @@
       <c r="H103" s="2">
         <v>-5.99148228472996</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I103" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
         <v>409</v>
       </c>
@@ -5256,8 +5555,11 @@
       <c r="H104" s="2">
         <v>-5.9910036196971701</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I104" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
         <v>412</v>
       </c>
@@ -5282,8 +5584,11 @@
       <c r="H105" s="2">
         <v>-5.9968748132764702</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I105" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
         <v>415</v>
       </c>
@@ -5308,8 +5613,11 @@
       <c r="H106" s="2">
         <v>-5.9951841205607899</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I106" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
         <v>419</v>
       </c>
@@ -5334,8 +5642,11 @@
       <c r="H107" s="2">
         <v>-5.9912808286271098</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I107" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
         <v>423</v>
       </c>
@@ -5360,8 +5671,11 @@
       <c r="H108" s="2">
         <v>-5.9909194290559604</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I108" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
         <v>427</v>
       </c>
@@ -5386,8 +5700,11 @@
       <c r="H110" s="2">
         <v>2.6341813114999102</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I110" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
         <v>432</v>
       </c>
@@ -5412,8 +5729,11 @@
       <c r="H111" s="2">
         <v>2.53738192708665</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I111" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
         <v>436</v>
       </c>
@@ -5438,8 +5758,11 @@
       <c r="H112" s="2">
         <v>3.0829410280687899</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I112" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
         <v>440</v>
       </c>
@@ -5464,8 +5787,11 @@
       <c r="H113" s="2">
         <v>3.0815864953705301</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I113" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
         <v>444</v>
       </c>
@@ -5490,8 +5816,11 @@
       <c r="H114" s="2">
         <v>2.6551848996344298</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I114" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
         <v>447</v>
       </c>
@@ -5516,8 +5845,11 @@
       <c r="H115" s="2">
         <v>2.6288887075327998</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I115" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
         <v>451</v>
       </c>
@@ -5542,8 +5874,11 @@
       <c r="H117" s="2">
         <v>-3.59711016142791</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I117" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
         <v>455</v>
       </c>
@@ -5568,8 +5903,11 @@
       <c r="H118" s="2">
         <v>-3.5997149435583999</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I118" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
         <v>459</v>
       </c>
@@ -5594,8 +5932,11 @@
       <c r="H119" s="2">
         <v>-3.6035236483931801</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I119" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A120" s="2" t="s">
         <v>463</v>
       </c>
@@ -5620,8 +5961,11 @@
       <c r="H120" s="2">
         <v>-3.5962655839570798</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I120" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A121" s="2" t="s">
         <v>467</v>
       </c>
@@ -5646,8 +5990,11 @@
       <c r="H121" s="2">
         <v>-3.5915755432508298</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I121" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A122" s="2" t="s">
         <v>470</v>
       </c>
@@ -5672,8 +6019,11 @@
       <c r="H122" s="2">
         <v>-3.5866711034850498</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I122" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A124" s="2" t="s">
         <v>474</v>
       </c>
@@ -5698,8 +6048,11 @@
       <c r="H124" s="2">
         <v>-4.7829954223035003</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I124" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A125" s="2" t="s">
         <v>478</v>
       </c>
@@ -5724,8 +6077,11 @@
       <c r="H125" s="2">
         <v>-4.7898892676020299</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I125" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A126" s="2" t="s">
         <v>484</v>
       </c>
@@ -5750,8 +6106,11 @@
       <c r="H126" s="2">
         <v>-4.7651563649203901</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I126" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A127" s="2" t="s">
         <v>489</v>
       </c>
@@ -5776,8 +6135,11 @@
       <c r="H127" s="2">
         <v>-4.7755422152814502</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I127" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A128" s="2" t="s">
         <v>491</v>
       </c>
@@ -5802,8 +6164,11 @@
       <c r="H128" s="2">
         <v>-4.7770106005879498</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I128" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A129" s="2" t="s">
         <v>493</v>
       </c>
@@ -5828,8 +6193,11 @@
       <c r="H129" s="2">
         <v>-4.7800025807987296</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I129" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A131" s="2" t="s">
         <v>497</v>
       </c>
@@ -5854,8 +6222,11 @@
       <c r="H131" s="2">
         <v>9.1816731756858694</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I131" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A132" s="2" t="s">
         <v>502</v>
       </c>
@@ -5880,8 +6251,11 @@
       <c r="H132" s="2">
         <v>9.1954315548432497</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I132" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A133" s="2" t="s">
         <v>506</v>
       </c>
@@ -5906,8 +6280,11 @@
       <c r="H133" s="2">
         <v>9.1904253092932997</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I133" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A134" s="2" t="s">
         <v>509</v>
       </c>
@@ -5932,8 +6309,11 @@
       <c r="H134" s="2">
         <v>9.1864112987956492</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I134" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A135" s="2" t="s">
         <v>512</v>
       </c>
@@ -5958,8 +6338,11 @@
       <c r="H135" s="2">
         <v>9.2079695462293891</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I135" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A136" s="2" t="s">
         <v>516</v>
       </c>
@@ -5984,15 +6367,18 @@
       <c r="H136" s="2">
         <v>9.1989617131293393</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I136" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A138" s="2" t="s">
         <v>518</v>
       </c>
@@ -6017,8 +6403,11 @@
       <c r="H138" s="2">
         <v>12.3378214095728</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I138" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A139" s="2" t="s">
         <v>522</v>
       </c>
@@ -6043,8 +6432,11 @@
       <c r="H139" s="2">
         <v>12.326541374367</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I139" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A140" s="2" t="s">
         <v>526</v>
       </c>
@@ -6069,8 +6461,11 @@
       <c r="H140" s="2">
         <v>12.351253619426799</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I140" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A141" s="2" t="s">
         <v>530</v>
       </c>
@@ -6095,8 +6490,11 @@
       <c r="H141" s="2">
         <v>12.3253742288959</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I141" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A142" s="2" t="s">
         <v>533</v>
       </c>
@@ -6121,8 +6519,11 @@
       <c r="H142" s="2">
         <v>12.3335173502989</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I142" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A143" s="2" t="s">
         <v>535</v>
       </c>
@@ -6147,8 +6548,11 @@
       <c r="H143" s="2">
         <v>12.3263729987688</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I143" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A145" s="2" t="s">
         <v>538</v>
       </c>
@@ -6173,8 +6577,11 @@
       <c r="H145" s="2">
         <v>11.2579638149542</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I145" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A146" s="2" t="s">
         <v>540</v>
       </c>
@@ -6199,8 +6606,11 @@
       <c r="H146" s="2">
         <v>11.253960911932101</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I146" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A147" s="2" t="s">
         <v>542</v>
       </c>
@@ -6225,8 +6635,11 @@
       <c r="H147" s="2">
         <v>11.254130490458699</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I147" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A148" s="2" t="s">
         <v>546</v>
       </c>
@@ -6251,8 +6664,11 @@
       <c r="H148" s="2">
         <v>11.2562291992285</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I148" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A149" s="2" t="s">
         <v>550</v>
       </c>
@@ -6277,8 +6693,11 @@
       <c r="H149" s="2">
         <v>11.2556823345219</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I149" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A150" s="2" t="s">
         <v>554</v>
       </c>
@@ -6303,8 +6722,11 @@
       <c r="H150" s="2">
         <v>11.2505652119606</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I150" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A152" s="2" t="s">
         <v>559</v>
       </c>
@@ -6329,8 +6751,11 @@
       <c r="H152" s="2">
         <v>12.4554670130539</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I152" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A153" s="2" t="s">
         <v>562</v>
       </c>
@@ -6355,8 +6780,11 @@
       <c r="H153" s="2">
         <v>12.453551680333</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I153" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A154" s="2" t="s">
         <v>566</v>
       </c>
@@ -6381,8 +6809,11 @@
       <c r="H154" s="2">
         <v>12.471605310150199</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I154" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A155" s="2" t="s">
         <v>570</v>
       </c>
@@ -6407,8 +6838,11 @@
       <c r="H155" s="2">
         <v>12.4844867529668</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I155" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A156" s="2" t="s">
         <v>573</v>
       </c>
@@ -6433,8 +6867,11 @@
       <c r="H156" s="2">
         <v>12.512203039362101</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I156" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A157" s="2" t="s">
         <v>576</v>
       </c>
@@ -6459,8 +6896,11 @@
       <c r="H157" s="2">
         <v>12.4657720641944</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I157" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A159" s="2" t="s">
         <v>581</v>
       </c>
@@ -6485,8 +6925,11 @@
       <c r="H159" s="2">
         <v>14.2764515744137</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I159" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A160" s="2" t="s">
         <v>586</v>
       </c>
@@ -6511,8 +6954,11 @@
       <c r="H160" s="2">
         <v>14.250539332730201</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I160" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A161" s="2" t="s">
         <v>590</v>
       </c>
@@ -6537,8 +6983,11 @@
       <c r="H161" s="2">
         <v>14.210898128537799</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I161" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A162" s="2" t="s">
         <v>594</v>
       </c>
@@ -6563,8 +7012,11 @@
       <c r="H162" s="2">
         <v>14.257152903033001</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I162" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A163" s="2" t="s">
         <v>598</v>
       </c>
@@ -6589,8 +7041,11 @@
       <c r="H163" s="2">
         <v>14.245252942038199</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I163" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A164" s="2" t="s">
         <v>603</v>
       </c>
@@ -6615,8 +7070,11 @@
       <c r="H164" s="2">
         <v>14.2346432948826</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I164" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A166" s="2" t="s">
         <v>607</v>
       </c>
@@ -6641,8 +7099,11 @@
       <c r="H166" s="2">
         <v>8.5858751274149601</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I166" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A167" s="2" t="s">
         <v>611</v>
       </c>
@@ -6667,8 +7128,11 @@
       <c r="H167" s="2">
         <v>8.5392598358265595</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I167" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A168" s="2" t="s">
         <v>616</v>
       </c>
@@ -6693,8 +7157,11 @@
       <c r="H168" s="2">
         <v>8.5430121501426193</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I168" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A169" s="2" t="s">
         <v>621</v>
       </c>
@@ -6719,8 +7186,11 @@
       <c r="H169" s="2">
         <v>8.5392845504703594</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I169" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A170" s="2" t="s">
         <v>626</v>
       </c>
@@ -6745,8 +7215,11 @@
       <c r="H170" s="2">
         <v>8.5099838407903103</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I170" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A171" s="2" t="s">
         <v>630</v>
       </c>
@@ -6771,8 +7244,11 @@
       <c r="H171" s="2">
         <v>8.5458399412155597</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I171" s="2" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A173" s="2" t="s">
         <v>634</v>
       </c>
@@ -6797,8 +7273,11 @@
       <c r="H173" s="2">
         <v>8.3078859314106897</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I173" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A174" s="2" t="s">
         <v>638</v>
       </c>
@@ -6823,8 +7302,11 @@
       <c r="H174" s="2">
         <v>8.3012702836466801</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I174" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A175" s="2" t="s">
         <v>643</v>
       </c>
@@ -6849,8 +7331,11 @@
       <c r="H175" s="2">
         <v>8.3093323535127901</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I175" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A176" s="2" t="s">
         <v>646</v>
       </c>
@@ -6875,8 +7360,11 @@
       <c r="H176" s="2">
         <v>8.3434752181485106</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I176" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A177" s="2" t="s">
         <v>651</v>
       </c>
@@ -6901,8 +7389,11 @@
       <c r="H177" s="2">
         <v>8.3196506030206798</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I177" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A178" s="2" t="s">
         <v>655</v>
       </c>
@@ -6927,8 +7418,11 @@
       <c r="H178" s="2">
         <v>8.3146905488973299</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I178" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A180" s="2" t="s">
         <v>660</v>
       </c>
@@ -6953,8 +7447,11 @@
       <c r="H180" s="2">
         <v>6.1497079215382104</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I180" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A181" s="2" t="s">
         <v>664</v>
       </c>
@@ -6979,8 +7476,11 @@
       <c r="H181" s="2">
         <v>6.14549228953436</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I181" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A182" s="2" t="s">
         <v>669</v>
       </c>
@@ -7005,8 +7505,11 @@
       <c r="H182" s="2">
         <v>6.1347396732208201</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I182" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A183" s="2" t="s">
         <v>674</v>
       </c>
@@ -7031,8 +7534,11 @@
       <c r="H183" s="2">
         <v>6.1484877391751898</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I183" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A184" s="2" t="s">
         <v>677</v>
       </c>
@@ -7057,8 +7563,11 @@
       <c r="H184" s="2">
         <v>6.1384499332115103</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I184" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A185" s="2" t="s">
         <v>680</v>
       </c>
@@ -7083,15 +7592,18 @@
       <c r="H185" s="2">
         <v>6.1518225274822003</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I185" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
       <c r="E186" s="1"/>
       <c r="F186" s="1"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A187" s="2" t="s">
         <v>685</v>
       </c>
@@ -7116,8 +7628,11 @@
       <c r="H187" s="2">
         <v>7.8703762666278703</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I187" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A188" s="2" t="s">
         <v>689</v>
       </c>
@@ -7142,8 +7657,11 @@
       <c r="H188" s="2">
         <v>7.8557247535002803</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I188" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A189" s="2" t="s">
         <v>693</v>
       </c>
@@ -7168,8 +7686,11 @@
       <c r="H189" s="2">
         <v>7.8546337700845701</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I189" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A190" s="2" t="s">
         <v>697</v>
       </c>
@@ -7194,8 +7715,11 @@
       <c r="H190" s="2">
         <v>7.8548693089006898</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I190" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A191" s="2" t="s">
         <v>702</v>
       </c>
@@ -7220,8 +7744,11 @@
       <c r="H191" s="2">
         <v>7.8185260964549999</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I191" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A192" s="2" t="s">
         <v>707</v>
       </c>
@@ -7246,8 +7773,11 @@
       <c r="H192" s="2">
         <v>7.8635395865401296</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I192" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A194" s="2" t="s">
         <v>711</v>
       </c>
@@ -7272,8 +7802,11 @@
       <c r="H194" s="2">
         <v>7.4566173791906003</v>
       </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I194" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A195" s="2" t="s">
         <v>715</v>
       </c>
@@ -7298,8 +7831,11 @@
       <c r="H195" s="2">
         <v>7.4496253296642196</v>
       </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I195" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A196" s="2" t="s">
         <v>718</v>
       </c>
@@ -7324,8 +7860,11 @@
       <c r="H196" s="2">
         <v>7.4282566998185002</v>
       </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I196" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A197" s="2" t="s">
         <v>722</v>
       </c>
@@ -7350,8 +7889,11 @@
       <c r="H197" s="2">
         <v>7.4575953648534004</v>
       </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I197" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A198" s="2" t="s">
         <v>726</v>
       </c>
@@ -7376,8 +7918,11 @@
       <c r="H198" s="2">
         <v>7.4487350948551301</v>
       </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I198" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A199" s="2" t="s">
         <v>730</v>
       </c>
@@ -7402,8 +7947,11 @@
       <c r="H199" s="2">
         <v>7.4470768507574698</v>
       </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I199" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A201" s="2" t="s">
         <v>734</v>
       </c>
@@ -7428,8 +7976,11 @@
       <c r="H201" s="2">
         <v>7.7470983447282</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I201" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A202" s="2" t="s">
         <v>738</v>
       </c>
@@ -7454,8 +8005,11 @@
       <c r="H202" s="2">
         <v>7.74852161022738</v>
       </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I202" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A203" s="2" t="s">
         <v>741</v>
       </c>
@@ -7480,8 +8034,11 @@
       <c r="H203" s="2">
         <v>7.7359727482711396</v>
       </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I203" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A204" s="2" t="s">
         <v>745</v>
       </c>
@@ -7506,8 +8063,11 @@
       <c r="H204" s="2">
         <v>7.7536372668484201</v>
       </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I204" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A205" s="2" t="s">
         <v>749</v>
       </c>
@@ -7532,8 +8092,11 @@
       <c r="H205" s="2">
         <v>7.75405470984147</v>
       </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I205" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A206" s="2" t="s">
         <v>753</v>
       </c>
@@ -7558,8 +8121,11 @@
       <c r="H206" s="2">
         <v>7.7675199521533198</v>
       </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I206" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A208" s="2" t="s">
         <v>756</v>
       </c>
@@ -7584,8 +8150,11 @@
       <c r="H208" s="2">
         <v>8.9603259113970299</v>
       </c>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I208" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A209" s="2" t="s">
         <v>760</v>
       </c>
@@ -7610,8 +8179,11 @@
       <c r="H209" s="2">
         <v>9.0022614874747493</v>
       </c>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I209" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A210" s="2" t="s">
         <v>764</v>
       </c>
@@ -7636,8 +8208,11 @@
       <c r="H210" s="2">
         <v>8.9453297580702191</v>
       </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I210" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A211" s="2" t="s">
         <v>768</v>
       </c>
@@ -7662,8 +8237,11 @@
       <c r="H211" s="2">
         <v>8.9701898502246706</v>
       </c>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I211" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A212" s="2" t="s">
         <v>772</v>
       </c>
@@ -7688,8 +8266,11 @@
       <c r="H212" s="2">
         <v>8.9295013772842395</v>
       </c>
-    </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I212" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A213" s="2" t="s">
         <v>776</v>
       </c>
@@ -7714,8 +8295,11 @@
       <c r="H213" s="2">
         <v>8.9437036192858095</v>
       </c>
-    </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I213" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A215" s="2" t="s">
         <v>780</v>
       </c>
@@ -7740,8 +8324,11 @@
       <c r="H215" s="2">
         <v>8.9679068443389998</v>
       </c>
-    </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I215" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A216" s="2" t="s">
         <v>768</v>
       </c>
@@ -7766,8 +8353,11 @@
       <c r="H216" s="2">
         <v>8.9701889224382505</v>
       </c>
-    </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I216" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A217" s="2" t="s">
         <v>784</v>
       </c>
@@ -7792,8 +8382,11 @@
       <c r="H217" s="2">
         <v>8.9497929519358195</v>
       </c>
-    </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I217" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A218" s="2" t="s">
         <v>788</v>
       </c>
@@ -7818,8 +8411,11 @@
       <c r="H218" s="2">
         <v>8.9457138030351508</v>
       </c>
-    </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I218" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A219" s="2" t="s">
         <v>792</v>
       </c>
@@ -7844,8 +8440,11 @@
       <c r="H219" s="2">
         <v>8.9560908289932204</v>
       </c>
-    </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I219" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A220" s="2" t="s">
         <v>796</v>
       </c>
@@ -7870,8 +8469,11 @@
       <c r="H220" s="2">
         <v>8.9571702983401806</v>
       </c>
-    </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I220" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A222" s="2" t="s">
         <v>800</v>
       </c>
@@ -7895,6 +8497,9 @@
       </c>
       <c r="H222" s="2">
         <v>8.3487811743276197</v>
+      </c>
+      <c r="I222" s="2" t="s">
+        <v>806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>